<commit_message>
Started two site DDL modeling
</commit_message>
<xml_diff>
--- a/Sorption Experiments/RaFHY_pH3/RaFHY_ph3_NoScript.xlsx
+++ b/Sorption Experiments/RaFHY_pH3/RaFHY_ph3_NoScript.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Dropbox (Personal)\work\MIT Graduate Work\Research\Radium Sorption\Sorption Experiments\RaFHY_pH3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Dropbox (Personal)\work\MIT Graduate Work\Research\RadiumSorption\Sorption Experiments\RaFHY_pH3\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="12285" firstSheet="3" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="12285" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="1" r:id="rId1"/>
@@ -10275,11 +10275,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="Q2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I10" sqref="I10"/>
+      <selection pane="bottomRight" activeCell="W12" sqref="W12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11738,8 +11738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K4:K5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Corrected all except RaFHY pH9
</commit_message>
<xml_diff>
--- a/Sorption Experiments/RaFHY_pH3/RaFHY_ph3_NoScript.xlsx
+++ b/Sorption Experiments/RaFHY_pH3/RaFHY_ph3_NoScript.xlsx
@@ -9,8 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="12285" firstSheet="3" activeTab="5"/>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" firstSheet="3" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="12285" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="1" r:id="rId1"/>
@@ -1014,9 +1013,6 @@
     <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6:C6"/>
     </sheetView>
-    <sheetView workbookViewId="1">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1116,7 +1112,6 @@
     <sheetView workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7634,10 +7629,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C2:C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -8407,7 +8401,6 @@
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -11116,12 +11109,6 @@
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="W15" sqref="W15"/>
-    </sheetView>
-    <sheetView tabSelected="1" workbookViewId="1">
-      <pane xSplit="1" ySplit="1" topLeftCell="Q2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q5" sqref="Q5:Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12580,11 +12567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
-    </sheetView>
-    <sheetView workbookViewId="1">
-      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>